<commit_message>
Updates for Appendix A example graphics
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Producer CONNECT" sheetId="2" r:id="rId1"/>
+    <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
     <sheet name="PUBLISH example" sheetId="1" r:id="rId2"/>
     <sheet name="zulu SUBSCRIBE" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -180,9 +180,6 @@
     <t>keepAlive</t>
   </si>
   <si>
-    <t>"orch01"</t>
-  </si>
-  <si>
     <t>"orch01north"</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>Ý</t>
   </si>
   <si>
-    <t>Windings: 221</t>
-  </si>
-  <si>
     <t>topicFilter</t>
   </si>
   <si>
@@ -229,6 +223,48 @@
   </si>
   <si>
     <t>"oc2/cmd/device/zulu1"</t>
+  </si>
+  <si>
+    <t>"zulu01north"</t>
+  </si>
+  <si>
+    <t>"=Pacific="</t>
+  </si>
+  <si>
+    <t>SUBACK</t>
+  </si>
+  <si>
+    <t>packetId</t>
+  </si>
+  <si>
+    <t>returnCode 1</t>
+  </si>
+  <si>
+    <t>returnCode 2</t>
+  </si>
+  <si>
+    <t>returnCode 3</t>
+  </si>
+  <si>
+    <t>returnCode 4</t>
+  </si>
+  <si>
+    <t>Ýþ</t>
+  </si>
+  <si>
+    <t>Windings: 221, 254</t>
+  </si>
+  <si>
+    <t>Þþ</t>
+  </si>
+  <si>
+    <t>PUBACK</t>
+  </si>
+  <si>
+    <t>"hzboblxic"</t>
+  </si>
+  <si>
+    <t>"smtwzzwvx"</t>
   </si>
 </sst>
 </file>
@@ -402,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -445,6 +481,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +562,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -834,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,10 +898,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -878,7 +917,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -894,7 +933,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
@@ -902,7 +941,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -919,17 +958,70 @@
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
+      <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="13">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,16 +1031,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E17"/>
+  <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -964,10 +1056,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -991,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1015,13 +1107,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
       <c r="C10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1041,14 +1133,38 @@
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="13">
+        <v>4314</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1059,7 +1175,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E18"/>
+  <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -1068,7 +1184,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1081,13 +1197,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1100,70 +1216,75 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="C5" s="10">
+        <v>47826</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="10">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C11" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
@@ -1171,14 +1292,70 @@
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="10">
+        <v>47826</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="13">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revise examples in Appendix A
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
@@ -873,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E20"/>
+  <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,71 +955,68 @@
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B14" s="6" t="s">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+    <row r="15" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10" t="b">
+      <c r="C16" s="10" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
+    <row r="19" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C19" s="13">
         <v>300</v>
       </c>
     </row>
@@ -1031,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,42 +1124,36 @@
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
+    <row r="17" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C17" s="13">
         <v>4314</v>
       </c>
     </row>
@@ -1175,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E24"/>
+  <dimension ref="B1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,45 +1280,50 @@
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B18" s="6" t="s">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="10">
+        <v>47826</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="10">
-        <v>47826</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="10">
         <v>1</v>
@@ -1335,25 +1331,17 @@
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="s">
+    <row r="23" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C23" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More MQTT 5.0 changes
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -108,9 +108,6 @@
     </r>
   </si>
   <si>
-    <t>cleanSession</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -265,6 +262,33 @@
   </si>
   <si>
     <t>"smtwzzwvx"</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  cleanStart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  userName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  willRetain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  willQoS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  willFlag</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  reserved</t>
   </si>
 </sst>
 </file>
@@ -438,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -484,6 +508,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +925,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -917,106 +944,211 @@
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="13">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C21" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B30" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="C30" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+    <row r="32" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="13">
+      <c r="C32" s="13">
         <v>300</v>
       </c>
     </row>
@@ -1030,7 +1162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1053,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1080,7 +1212,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1104,13 +1236,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1135,10 +1267,10 @@
     </row>
     <row r="15" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1188,13 +1320,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1207,7 +1339,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="10">
         <v>47826</v>
@@ -1215,10 +1347,10 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1231,10 +1363,10 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1247,10 +1379,10 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1263,10 +1395,10 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1291,10 +1423,10 @@
     </row>
     <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -1307,7 +1439,7 @@
     </row>
     <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="10">
         <v>47826</v>
@@ -1315,7 +1447,7 @@
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="10">
         <v>1</v>
@@ -1323,7 +1455,7 @@
     </row>
     <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="10">
         <v>1</v>
@@ -1331,7 +1463,7 @@
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="10">
         <v>1</v>
@@ -1339,7 +1471,7 @@
     </row>
     <row r="23" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="13">
         <v>1</v>

</xml_diff>

<commit_message>
Update sub / suback image file
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -234,18 +234,6 @@
     <t>packetId</t>
   </si>
   <si>
-    <t>returnCode 1</t>
-  </si>
-  <si>
-    <t>returnCode 2</t>
-  </si>
-  <si>
-    <t>returnCode 3</t>
-  </si>
-  <si>
-    <t>returnCode 4</t>
-  </si>
-  <si>
     <t>Ýþ</t>
   </si>
   <si>
@@ -289,6 +277,36 @@
   </si>
   <si>
     <t xml:space="preserve">  reserved</t>
+  </si>
+  <si>
+    <t>SubscriptionOptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  maxQoS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  RH</t>
+  </si>
+  <si>
+    <t>reasonCode 1</t>
+  </si>
+  <si>
+    <t>reasonCode 2</t>
+  </si>
+  <si>
+    <t>reasonCode 3</t>
+  </si>
+  <si>
+    <t>reasonCode 4</t>
+  </si>
+  <si>
+    <t>Windings: 222, 254</t>
   </si>
 </sst>
 </file>
@@ -589,8 +607,8 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
@@ -902,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,18 +962,18 @@
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
@@ -963,7 +981,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -971,7 +989,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
@@ -979,7 +997,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -987,7 +1005,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -995,7 +1013,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -1003,7 +1021,7 @@
     </row>
     <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
@@ -1063,18 +1081,18 @@
         <v>11</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23" s="10">
         <v>1</v>
@@ -1082,7 +1100,7 @@
     </row>
     <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="10">
         <v>1</v>
@@ -1090,7 +1108,7 @@
     </row>
     <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C25" s="10">
         <v>0</v>
@@ -1098,15 +1116,15 @@
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C27" s="10">
         <v>0</v>
@@ -1114,7 +1132,7 @@
     </row>
     <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" s="10">
         <v>0</v>
@@ -1122,7 +1140,7 @@
     </row>
     <row r="29" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
@@ -1163,7 +1181,7 @@
   <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1206,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1267,10 +1285,10 @@
     </row>
     <row r="15" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1298,17 +1316,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E23"/>
+  <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1355,23 +1373,21 @@
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10">
-        <v>1</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C9" s="10">
         <v>1</v>
@@ -1379,18 +1395,18 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C11" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1398,64 +1414,72 @@
         <v>26</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>3</v>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="10">
-        <v>47826</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C20" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C21" s="10">
         <v>1</v>
@@ -1463,22 +1487,140 @@
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C22" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="13">
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="10">
+        <v>47826</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update pub / puback example messages image
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -41,13 +41,7 @@
     <t>qos</t>
   </si>
   <si>
-    <t>retainFlag</t>
-  </si>
-  <si>
     <t>payload</t>
-  </si>
-  <si>
-    <t>dupFlag</t>
   </si>
   <si>
     <r>
@@ -192,9 +186,6 @@
     <t>"oc2/cmd/ap/iota"</t>
   </si>
   <si>
-    <t>0x90 0x01</t>
-  </si>
-  <si>
     <t>"(JSON-encoded openc2 request)"</t>
   </si>
   <si>
@@ -307,6 +298,45 @@
   </si>
   <si>
     <t>Windings: 222, 254</t>
+  </si>
+  <si>
+    <t>dup</t>
+  </si>
+  <si>
+    <t>0 (false)</t>
+  </si>
+  <si>
+    <t>retain</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  propertyLength</t>
+  </si>
+  <si>
+    <t>(computed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  payloadFormat</t>
+  </si>
+  <si>
+    <t>"req"</t>
+  </si>
+  <si>
+    <t>"json"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  up: "msgType"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  up: "encoding"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  contentType</t>
+  </si>
+  <si>
+    <t>"application/openc2"</t>
   </si>
 </sst>
 </file>
@@ -553,8 +583,8 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
@@ -940,13 +970,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -959,21 +989,21 @@
     </row>
     <row r="5" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
@@ -981,7 +1011,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -989,7 +1019,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
@@ -997,7 +1027,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -1005,7 +1035,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -1013,7 +1043,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -1021,7 +1051,7 @@
     </row>
     <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
@@ -1029,23 +1059,23 @@
     </row>
     <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="13">
         <v>300</v>
@@ -1062,10 +1092,10 @@
     </row>
     <row r="19" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1078,21 +1108,21 @@
     </row>
     <row r="21" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C23" s="10">
         <v>1</v>
@@ -1100,7 +1130,7 @@
     </row>
     <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C24" s="10">
         <v>1</v>
@@ -1108,7 +1138,7 @@
     </row>
     <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="10">
         <v>0</v>
@@ -1116,15 +1146,15 @@
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C27" s="10">
         <v>0</v>
@@ -1132,7 +1162,7 @@
     </row>
     <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C28" s="10">
         <v>0</v>
@@ -1140,7 +1170,7 @@
     </row>
     <row r="29" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
@@ -1148,23 +1178,23 @@
     </row>
     <row r="30" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C32" s="13">
         <v>300</v>
@@ -1178,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E17"/>
+  <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1219,7 +1249,7 @@
     </row>
     <row r="5" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="10">
         <v>4314</v>
@@ -1227,83 +1257,124 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="10">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10" t="b">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="13">
+      <c r="C22" s="13">
         <v>4314</v>
       </c>
     </row>
@@ -1318,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1338,13 +1409,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1357,7 +1428,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" s="10">
         <v>47826</v>
@@ -1365,21 +1436,21 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" s="10">
         <v>2</v>
@@ -1387,7 +1458,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" s="10">
         <v>1</v>
@@ -1395,7 +1466,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -1403,7 +1474,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -1411,21 +1482,21 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="10">
         <v>2</v>
@@ -1433,7 +1504,7 @@
     </row>
     <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C15" s="10">
         <v>1</v>
@@ -1441,7 +1512,7 @@
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16" s="10">
         <v>1</v>
@@ -1449,7 +1520,7 @@
     </row>
     <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" s="10">
         <v>0</v>
@@ -1457,21 +1528,21 @@
     </row>
     <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="10"/>
     </row>
     <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C20" s="10">
         <v>2</v>
@@ -1479,7 +1550,7 @@
     </row>
     <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="10">
         <v>1</v>
@@ -1487,7 +1558,7 @@
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="10">
         <v>1</v>
@@ -1495,7 +1566,7 @@
     </row>
     <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" s="10">
         <v>0</v>
@@ -1503,21 +1574,21 @@
     </row>
     <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C26" s="10">
         <v>2</v>
@@ -1525,7 +1596,7 @@
     </row>
     <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C27" s="10">
         <v>1</v>
@@ -1533,7 +1604,7 @@
     </row>
     <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C28" s="10">
         <v>1</v>
@@ -1541,7 +1612,7 @@
     </row>
     <row r="29" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C29" s="13">
         <v>0</v>
@@ -1561,13 +1632,13 @@
     </row>
     <row r="33" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B33" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1580,7 +1651,7 @@
     </row>
     <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35" s="10">
         <v>47826</v>
@@ -1588,7 +1659,7 @@
     </row>
     <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C36" s="10">
         <v>2</v>
@@ -1596,7 +1667,7 @@
     </row>
     <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C37" s="10">
         <v>2</v>
@@ -1604,7 +1675,7 @@
     </row>
     <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C38" s="10">
         <v>2</v>
@@ -1612,7 +1683,7 @@
     </row>
     <row r="39" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C39" s="13">
         <v>2</v>

</xml_diff>

<commit_message>
Continuing MQTT v5.0 updates
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>topicName</t>
-  </si>
-  <si>
-    <t>qos</t>
   </si>
   <si>
     <t>payload</t>
@@ -270,21 +267,6 @@
     <t xml:space="preserve">  reserved</t>
   </si>
   <si>
-    <t>SubscriptionOptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  maxQoS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  RAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  RH</t>
-  </si>
-  <si>
     <t>reasonCode 1</t>
   </si>
   <si>
@@ -300,50 +282,62 @@
     <t>Windings: 222, 254</t>
   </si>
   <si>
-    <t>dup</t>
-  </si>
-  <si>
-    <t>0 (false)</t>
-  </si>
-  <si>
-    <t>retain</t>
-  </si>
-  <si>
     <t>properties</t>
   </si>
   <si>
-    <t xml:space="preserve">  propertyLength</t>
-  </si>
-  <si>
-    <t>(computed)</t>
-  </si>
-  <si>
     <t xml:space="preserve">  payloadFormat</t>
   </si>
   <si>
-    <t>"req"</t>
-  </si>
-  <si>
-    <t>"json"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  up: "msgType"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  up: "encoding"</t>
-  </si>
-  <si>
     <t xml:space="preserve">  contentType</t>
   </si>
   <si>
     <t>"application/openc2"</t>
+  </si>
+  <si>
+    <t>1 (UTF-8 string)</t>
+  </si>
+  <si>
+    <t>"msgType:req"</t>
+  </si>
+  <si>
+    <t>"encoding:json"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  userProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  maxQoS=2, NL=1, RAP=1, RH=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  subOptions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">packetId </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>(always 0 for qos 0)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  flags</t>
+  </si>
+  <si>
+    <t>qos=1, dup=0, retain=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +398,13 @@
       <color theme="1"/>
       <name val="Wingdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -510,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -559,6 +560,13 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,7 +591,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -637,7 +645,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -970,13 +978,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -989,21 +997,21 @@
     </row>
     <row r="5" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
@@ -1011,7 +1019,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="10">
         <v>1</v>
@@ -1019,7 +1027,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
@@ -1027,7 +1035,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -1035,7 +1043,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -1043,7 +1051,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
@@ -1051,7 +1059,7 @@
     </row>
     <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
@@ -1059,23 +1067,23 @@
     </row>
     <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="13">
         <v>300</v>
@@ -1092,10 +1100,10 @@
     </row>
     <row r="19" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1108,21 +1116,21 @@
     </row>
     <row r="21" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="10">
         <v>1</v>
@@ -1130,7 +1138,7 @@
     </row>
     <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="10">
         <v>1</v>
@@ -1138,7 +1146,7 @@
     </row>
     <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="10">
         <v>0</v>
@@ -1146,15 +1154,15 @@
     </row>
     <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="10">
         <v>0</v>
@@ -1162,7 +1170,7 @@
     </row>
     <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="10">
         <v>0</v>
@@ -1170,7 +1178,7 @@
     </row>
     <row r="29" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
@@ -1178,23 +1186,23 @@
     </row>
     <row r="30" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" s="13">
         <v>300</v>
@@ -1208,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E22"/>
+  <dimension ref="B1:O19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,27 +1227,28 @@
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="7" max="14" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1247,138 +1256,148 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
-        <v>7</v>
+    <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="C5" s="10">
         <v>4314</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="17"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="13">
+      <c r="C19" s="13">
         <v>4314</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="L8:M8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1387,17 +1406,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E39"/>
+  <dimension ref="B1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1409,13 +1428,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1428,7 +1447,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="10">
         <v>47826</v>
@@ -1436,256 +1455,136 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="10">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="10">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="10">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="10">
+    <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C19" s="10">
+        <v>47826</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B33" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="10">
-        <v>47826</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="13">
+      <c r="C23" s="13">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create Example 3 in Appendix A
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
     <sheet name="PUBLISH example" sheetId="1" r:id="rId2"/>
     <sheet name="zulu SUBSCRIBE" sheetId="3" r:id="rId3"/>
+    <sheet name="A3-query-all-profiles" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="73">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -332,12 +333,42 @@
   <si>
     <t>"zulu01"</t>
   </si>
+  <si>
+    <t>{"headers":{"request_id":"abc123","created":1610483633,"from":"Consumer1@example.com"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":["slpf"]}}}}}</t>
+  </si>
+  <si>
+    <t>Producer request for Consumer Aps</t>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"abc123","created":1610483630,"from":"Producer1@example.com"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
+  </si>
+  <si>
+    <t>Consumer 1 Response</t>
+  </si>
+  <si>
+    <t>"oc2/rsp"</t>
+  </si>
+  <si>
+    <t>"msgType:rsp"</t>
+  </si>
+  <si>
+    <t>Consumer 2 Response</t>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"Consumer2@example.com"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":["slpf","ids"]}}}}}</t>
+  </si>
+  <si>
+    <t>Consumer 3 Response</t>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"Consumer3@example.com"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":["edr","sbom"]}}}}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +436,28 @@
       <color theme="2" tint="-0.249977111117893"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -567,6 +620,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,6 +726,207 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5614987" y="2157412"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="2952750"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="2952750"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="3743325"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="3743325"/>
           <a:ext cx="65" cy="172227"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -958,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -1219,7 +1489,7 @@
   <dimension ref="B1:O19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,13 +1566,13 @@
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="18"/>
       <c r="O8" s="17"/>
     </row>
@@ -1593,4 +1863,590 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:O64"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="7" max="14" width="7.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="17"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="18" spans="2:15" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="24"/>
+    </row>
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10">
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="17"/>
+    </row>
+    <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="17"/>
+    </row>
+    <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+    </row>
+    <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="22"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="2:15" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="24"/>
+    </row>
+    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="10">
+        <v>9876</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="17"/>
+    </row>
+    <row r="42" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="17"/>
+    </row>
+    <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+    </row>
+    <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="22"/>
+    </row>
+    <row r="50" spans="2:15" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="24"/>
+    </row>
+    <row r="51" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="5"/>
+    </row>
+    <row r="53" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B53" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="10">
+        <v>6294</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" s="17"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="17"/>
+    </row>
+    <row r="58" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="10"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="17"/>
+    </row>
+    <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+    </row>
+    <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="10"/>
+    </row>
+    <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add disclaimer in Appendix re: from and to fields
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -334,15 +334,9 @@
     <t>"zulu01"</t>
   </si>
   <si>
-    <t>{"headers":{"request_id":"abc123","created":1610483633,"from":"Consumer1@example.com"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":["slpf"]}}}}}</t>
-  </si>
-  <si>
     <t>Producer request for Consumer Aps</t>
   </si>
   <si>
-    <t>{"headers":{"request_id":"abc123","created":1610483630,"from":"Producer1@example.com"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
-  </si>
-  <si>
     <t>Consumer 1 Response</t>
   </si>
   <si>
@@ -355,20 +349,153 @@
     <t>Consumer 2 Response</t>
   </si>
   <si>
-    <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"Consumer2@example.com"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":["slpf","ids"]}}}}}</t>
-  </si>
-  <si>
     <t>Consumer 3 Response</t>
   </si>
   <si>
-    <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"Consumer3@example.com"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":["edr","sbom"]}}}}}</t>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483630,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Producer1@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer3@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"edr","sbom"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer2@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"slpf","ids"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483633,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer1@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"slpf"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,18 +573,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -564,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -621,21 +759,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,13 +1707,13 @@
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
       <c r="N8" s="18"/>
       <c r="O8" s="17"/>
     </row>
@@ -1869,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,8 +2023,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
-        <v>64</v>
+      <c r="B1" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1916,7 +2057,7 @@
       <c r="B6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="24">
         <v>2468</v>
       </c>
     </row>
@@ -1932,7 +2073,7 @@
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="17"/>
@@ -1952,13 +2093,13 @@
       </c>
       <c r="C9" s="10"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
       <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="19"/>
       <c r="O9" s="17"/>
     </row>
@@ -1984,7 +2125,7 @@
       <c r="B11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="24" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2011,19 +2152,19 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="22"/>
+      <c r="B15" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
-    <row r="18" spans="2:15" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="24"/>
+    <row r="18" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="21"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -2055,7 +2196,7 @@
       <c r="B23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="24">
         <v>3571</v>
       </c>
     </row>
@@ -2071,8 +2212,8 @@
       <c r="B25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>67</v>
+      <c r="C25" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="19"/>
@@ -2091,13 +2232,13 @@
       </c>
       <c r="C26" s="10"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
       <c r="N26" s="19"/>
       <c r="O26" s="17"/>
     </row>
@@ -2123,8 +2264,8 @@
       <c r="B28" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>68</v>
+      <c r="C28" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2150,19 +2291,19 @@
       <c r="C31" s="10"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="22"/>
+      <c r="B32" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="26"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:15" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="24"/>
+    <row r="34" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="21"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
@@ -2194,7 +2335,7 @@
       <c r="B39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="24">
         <v>9876</v>
       </c>
     </row>
@@ -2210,8 +2351,8 @@
       <c r="B41" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>67</v>
+      <c r="C41" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="19"/>
@@ -2230,13 +2371,13 @@
       </c>
       <c r="C42" s="10"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
       <c r="N42" s="19"/>
       <c r="O42" s="17"/>
     </row>
@@ -2262,8 +2403,8 @@
       <c r="B44" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>68</v>
+      <c r="C44" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2289,16 +2430,16 @@
       <c r="C47" s="10"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="22"/>
-    </row>
-    <row r="50" spans="2:15" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="25" t="s">
+      <c r="B48" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="24"/>
+      <c r="C48" s="26"/>
+    </row>
+    <row r="50" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="21"/>
     </row>
     <row r="51" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
@@ -2330,7 +2471,7 @@
       <c r="B55" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="24">
         <v>6294</v>
       </c>
     </row>
@@ -2346,8 +2487,8 @@
       <c r="B57" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>67</v>
+      <c r="C57" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="19"/>
@@ -2366,13 +2507,13 @@
       </c>
       <c r="C58" s="10"/>
       <c r="F58" s="17"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="23"/>
       <c r="K58" s="19"/>
-      <c r="L58" s="20"/>
-      <c r="M58" s="20"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="23"/>
       <c r="N58" s="19"/>
       <c r="O58" s="17"/>
     </row>
@@ -2398,8 +2539,8 @@
       <c r="B60" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="10" t="s">
-        <v>68</v>
+      <c r="C60" s="24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2425,13 +2566,18 @@
       <c r="C63" s="10"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="22"/>
+      <c r="B64" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -2439,11 +2585,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Color highlights for example 3 packets
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -334,9 +334,6 @@
     <t>"zulu01"</t>
   </si>
   <si>
-    <t>Producer request for Consumer Aps</t>
-  </si>
-  <si>
     <t>Consumer 1 Response</t>
   </si>
   <si>
@@ -489,6 +486,9 @@
       </rPr>
       <t>]}}}}}</t>
     </r>
+  </si>
+  <si>
+    <t>Producer request for Consumer APs</t>
   </si>
 </sst>
 </file>
@@ -766,11 +766,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1707,13 +1707,13 @@
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="18"/>
       <c r="O8" s="17"/>
     </row>
@@ -2010,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2024,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="22" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2057,7 +2057,7 @@
       <c r="B6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>2468</v>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="17"/>
@@ -2093,13 +2093,13 @@
       </c>
       <c r="C9" s="10"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="19"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
       <c r="N9" s="19"/>
       <c r="O9" s="17"/>
     </row>
@@ -2125,7 +2125,7 @@
       <c r="B11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="26"/>
     </row>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="18" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="21"/>
     </row>
@@ -2196,7 +2196,7 @@
       <c r="B23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="23">
         <v>3571</v>
       </c>
     </row>
@@ -2212,8 +2212,8 @@
       <c r="B25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>65</v>
+      <c r="C25" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="19"/>
@@ -2232,13 +2232,13 @@
       </c>
       <c r="C26" s="10"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
       <c r="N26" s="19"/>
       <c r="O26" s="17"/>
     </row>
@@ -2264,8 +2264,8 @@
       <c r="B28" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>66</v>
+      <c r="C28" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2292,7 +2292,7 @@
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="26"/>
     </row>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="34" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="21"/>
     </row>
@@ -2335,7 +2335,7 @@
       <c r="B39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="23">
         <v>9876</v>
       </c>
     </row>
@@ -2351,8 +2351,8 @@
       <c r="B41" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>65</v>
+      <c r="C41" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="19"/>
@@ -2371,13 +2371,13 @@
       </c>
       <c r="C42" s="10"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
       <c r="N42" s="19"/>
       <c r="O42" s="17"/>
     </row>
@@ -2403,8 +2403,8 @@
       <c r="B44" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="24" t="s">
-        <v>66</v>
+      <c r="C44" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2431,13 +2431,13 @@
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="26"/>
     </row>
     <row r="50" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="21"/>
     </row>
@@ -2471,7 +2471,7 @@
       <c r="B55" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="23">
         <v>6294</v>
       </c>
     </row>
@@ -2487,8 +2487,8 @@
       <c r="B57" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="24" t="s">
-        <v>65</v>
+      <c r="C57" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="19"/>
@@ -2507,13 +2507,13 @@
       </c>
       <c r="C58" s="10"/>
       <c r="F58" s="17"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
       <c r="K58" s="19"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="23"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
       <c r="N58" s="19"/>
       <c r="O58" s="17"/>
     </row>
@@ -2539,8 +2539,8 @@
       <c r="B60" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="24" t="s">
-        <v>66</v>
+      <c r="C60" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2567,17 +2567,12 @@
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -2585,6 +2580,11 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Clean up connect packets graphic
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,6 +1622,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C26" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2010,7 +2013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2573,6 +2576,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -2580,11 +2588,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial pass reorganizing to new OASIS outline
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -307,6 +307,184 @@
     <t xml:space="preserve">  subOptions</t>
   </si>
   <si>
+    <t xml:space="preserve">  flags</t>
+  </si>
+  <si>
+    <t>qos=1, dup=0, retain=0</t>
+  </si>
+  <si>
+    <t>"orch01"</t>
+  </si>
+  <si>
+    <t>"zulu01"</t>
+  </si>
+  <si>
+    <t>Consumer 1 Response</t>
+  </si>
+  <si>
+    <t>"oc2/rsp"</t>
+  </si>
+  <si>
+    <t>"msgType:rsp"</t>
+  </si>
+  <si>
+    <t>Consumer 2 Response</t>
+  </si>
+  <si>
+    <t>Consumer 3 Response</t>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483630,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Producer1@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer3@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"edr","sbom"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer2@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"slpf","ids"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"abc123","created":1610483633,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer1@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"slpf"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <t>Producer request for Consumer APs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optional (O) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">suggested (S) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">required (R) </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">packetId </t>
     </r>
@@ -318,177 +496,8 @@
         <rFont val="Lucida Console"/>
         <family val="3"/>
       </rPr>
-      <t>(always 0 for qos 0)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  flags</t>
-  </si>
-  <si>
-    <t>qos=1, dup=0, retain=0</t>
-  </si>
-  <si>
-    <t>"orch01"</t>
-  </si>
-  <si>
-    <t>"zulu01"</t>
-  </si>
-  <si>
-    <t>Consumer 1 Response</t>
-  </si>
-  <si>
-    <t>"oc2/rsp"</t>
-  </si>
-  <si>
-    <t>"msgType:rsp"</t>
-  </si>
-  <si>
-    <t>Consumer 2 Response</t>
-  </si>
-  <si>
-    <t>Consumer 3 Response</t>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483630,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Producer1@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Consumer3@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"edr","sbom"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Consumer2@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"slpf","ids"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483633,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Consumer1@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"slpf"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <t>Producer request for Consumer APs</t>
+      <t>(=0 for QoS 0)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -598,12 +607,42 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -702,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -777,6 +816,45 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1367,27 +1445,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E32"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
@@ -1398,7 +1475,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1406,97 +1483,106 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="37" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="H6" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="H7" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="34">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+      <c r="C14" s="34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="30">
         <v>300</v>
       </c>
     </row>
@@ -1600,7 +1686,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -1633,13 +1719,13 @@
   <dimension ref="B1:O19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
     <col min="7" max="14" width="7.28515625" customWidth="1"/>
   </cols>
@@ -1672,25 +1758,25 @@
     </row>
     <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C5" s="10">
         <v>4314</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="17"/>
@@ -1721,10 +1807,10 @@
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="37" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="17"/>
@@ -1739,26 +1825,26 @@
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="37" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="37" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="37" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1769,8 +1855,8 @@
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="28" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2013,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2113,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2066,10 +2152,10 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2156,7 +2242,7 @@
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="26"/>
     </row>
@@ -2165,7 +2251,7 @@
     </row>
     <row r="18" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="21"/>
     </row>
@@ -2205,10 +2291,10 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2216,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="19"/>
@@ -2268,7 +2354,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2295,7 +2381,7 @@
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="26"/>
     </row>
@@ -2304,7 +2390,7 @@
     </row>
     <row r="34" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="21"/>
     </row>
@@ -2344,10 +2430,10 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2355,7 +2441,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="19"/>
@@ -2407,7 +2493,7 @@
         <v>55</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2434,13 +2520,13 @@
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="26"/>
     </row>
     <row r="50" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C50" s="21"/>
     </row>
@@ -2480,10 +2566,10 @@
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2491,7 +2577,7 @@
         <v>4</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="19"/>
@@ -2543,7 +2629,7 @@
         <v>55</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -2570,17 +2656,12 @@
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -2588,6 +2669,11 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add JSON, images to E.4 Deny example
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
     <sheet name="PUBLISH example" sheetId="1" r:id="rId2"/>
     <sheet name="zulu SUBSCRIBE" sheetId="3" r:id="rId3"/>
-    <sheet name="A3-query-all-profiles" sheetId="4" r:id="rId4"/>
+    <sheet name="E3-query-all-profiles" sheetId="4" r:id="rId4"/>
+    <sheet name="E4-deny-example" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="81">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -499,12 +500,27 @@
       <t>(=0 for QoS 0)</t>
     </r>
   </si>
+  <si>
+    <t>Producer request with SLPF `deny` action</t>
+  </si>
+  <si>
+    <t>"oc2/cmd/splf"</t>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"ghk479","created":1610483630,"from":"Producer1@example.com"},"body":{"openc2":{"request":{"action":"deny","target":{"ipv4_connection":{"protocol":"tcp","src_addr":"1.2.3.4","src_port":10996,"dst_addr":"198.2.3.4","dst_port":80}},"args":{"start_time":1534775460000,"duration":500,"response_requested":"ack","slpf":{"drop_process":"none"}},"actuator":{"slpf":{"asset_id":"30"}}}}}}</t>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"ghk479","created":1610483633,"from":"Consumer1@example.com"},"body":{"openc2":{"response":{"status":102}}}}</t>
+  </si>
+  <si>
+    <t>Consumer 1 Response to `deny` Request</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +619,17 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
@@ -741,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -810,12 +837,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -854,6 +875,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1182,6 +1218,207 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="4143375"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="4143375"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="8639175"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6053137" y="8639175"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1447,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1484,13 +1721,13 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="36" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1499,90 +1736,90 @@
         <v>34</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="29" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="32">
         <v>1</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="32" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="28">
         <v>300</v>
       </c>
     </row>
@@ -1765,18 +2002,18 @@
       </c>
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="35" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="17"/>
@@ -1796,21 +2033,21 @@
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
       <c r="N8" s="18"/>
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="35" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="17"/>
@@ -1825,26 +2062,26 @@
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="35" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="35" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="35" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1855,8 +2092,8 @@
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2182,13 +2419,13 @@
       </c>
       <c r="C9" s="10"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="19"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
       <c r="N9" s="19"/>
       <c r="O9" s="17"/>
     </row>
@@ -2241,10 +2478,10 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="42"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -2321,13 +2558,13 @@
       </c>
       <c r="C26" s="10"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
       <c r="N26" s="19"/>
       <c r="O26" s="17"/>
     </row>
@@ -2380,10 +2617,10 @@
       <c r="C31" s="10"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="26"/>
+      <c r="C32" s="42"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
@@ -2460,13 +2697,13 @@
       </c>
       <c r="C42" s="10"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="40"/>
       <c r="N42" s="19"/>
       <c r="O42" s="17"/>
     </row>
@@ -2519,10 +2756,10 @@
       <c r="C47" s="10"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="42"/>
     </row>
     <row r="50" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="22" t="s">
@@ -2596,13 +2833,13 @@
       </c>
       <c r="C58" s="10"/>
       <c r="F58" s="17"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
       <c r="K58" s="19"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="24"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="40"/>
       <c r="N58" s="19"/>
       <c r="O58" s="17"/>
     </row>
@@ -2655,13 +2892,18 @@
       <c r="C63" s="10"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="26"/>
+      <c r="C64" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -2669,11 +2911,314 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:O33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="7" max="14" width="7.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="44">
+        <v>62874</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="17"/>
+    </row>
+    <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="17"/>
+    </row>
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="42"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="18" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="2:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="44">
+        <v>87356</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="17"/>
+    </row>
+    <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="44"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="17"/>
+    </row>
+    <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+    </row>
+    <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="42"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add color code explanation, example
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -7,11 +7,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683"/>
   </bookViews>
   <sheets>
-    <sheet name="CONNECT Examples" sheetId="2" r:id="rId1"/>
-    <sheet name="PUBLISH example" sheetId="1" r:id="rId2"/>
-    <sheet name="zulu SUBSCRIBE" sheetId="3" r:id="rId3"/>
-    <sheet name="E3-query-all-profiles" sheetId="4" r:id="rId4"/>
-    <sheet name="E4-deny-example" sheetId="6" r:id="rId5"/>
+    <sheet name="color code" sheetId="7" r:id="rId1"/>
+    <sheet name="CONNECT Examples" sheetId="2" r:id="rId2"/>
+    <sheet name="PUBLISH example" sheetId="1" r:id="rId3"/>
+    <sheet name="zulu SUBSCRIBE" sheetId="3" r:id="rId4"/>
+    <sheet name="E3-query-all-profiles" sheetId="4" r:id="rId5"/>
+    <sheet name="E4-deny-example" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="89">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -828,7 +829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -920,11 +921,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1018,15 +1034,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1070,6 +1077,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,10 +1886,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:C7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,238 +1935,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="39"/>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="46" t="s">
+      <c r="A4" s="36"/>
+      <c r="B4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="38" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="34">
         <v>1</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="48" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="38" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="34">
         <v>1</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="38" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="34">
         <v>0</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="38" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="34">
         <v>0</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="38" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="34">
         <v>0</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="38" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="34">
         <v>0</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="38" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="37">
+      <c r="C13" s="34">
         <v>0</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
     </row>
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="36"/>
+      <c r="B15" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="49" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="47">
         <v>300</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -2235,7 +2293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O19"/>
   <sheetViews>
@@ -2317,13 +2375,13 @@
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
       <c r="K8" s="18"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
       <c r="N8" s="18"/>
       <c r="O8" s="17"/>
     </row>
@@ -2425,7 +2483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E23"/>
   <sheetViews>
@@ -2616,7 +2674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
@@ -2703,13 +2761,13 @@
       </c>
       <c r="C9" s="10"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
       <c r="K9" s="19"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
       <c r="N9" s="19"/>
       <c r="O9" s="17"/>
     </row>
@@ -2762,10 +2820,10 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="51"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -2842,13 +2900,13 @@
       </c>
       <c r="C26" s="10"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
       <c r="N26" s="19"/>
       <c r="O26" s="17"/>
     </row>
@@ -2901,10 +2959,10 @@
       <c r="C31" s="10"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="35"/>
+      <c r="C32" s="51"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
@@ -2981,13 +3039,13 @@
       </c>
       <c r="C42" s="10"/>
       <c r="F42" s="17"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="33"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
       <c r="K42" s="19"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
       <c r="N42" s="19"/>
       <c r="O42" s="17"/>
     </row>
@@ -3040,10 +3098,10 @@
       <c r="C47" s="10"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="35"/>
+      <c r="C48" s="51"/>
     </row>
     <row r="50" spans="2:15" s="20" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="22" t="s">
@@ -3117,13 +3175,13 @@
       </c>
       <c r="C58" s="10"/>
       <c r="F58" s="17"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
       <c r="K58" s="19"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
+      <c r="L58" s="49"/>
+      <c r="M58" s="49"/>
       <c r="N58" s="19"/>
       <c r="O58" s="17"/>
     </row>
@@ -3176,13 +3234,18 @@
       <c r="C63" s="10"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="35"/>
+      <c r="C64" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3190,11 +3253,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3202,7 +3260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O33"/>
   <sheetViews>
@@ -3289,13 +3347,13 @@
       </c>
       <c r="C9" s="32"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
       <c r="K9" s="24"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
       <c r="N9" s="24"/>
       <c r="O9" s="17"/>
     </row>
@@ -3348,10 +3406,10 @@
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="51"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -3428,13 +3486,13 @@
       </c>
       <c r="C26" s="32"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
       <c r="K26" s="24"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
       <c r="N26" s="24"/>
       <c r="O26" s="17"/>
     </row>
@@ -3487,10 +3545,10 @@
       <c r="C31" s="10"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="35"/>
+      <c r="C32" s="51"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>

</xml_diff>

<commit_message>
color example 3 packets
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="color code" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="92">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -758,6 +758,37 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> (s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  flags</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (r)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  userProperty (r)</t>
+  </si>
+  <si>
+    <r>
+      <t>payload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (r)</t>
     </r>
   </si>
 </sst>
@@ -1016,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1170,6 +1201,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2563,7 +2603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -2754,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2806,18 +2846,18 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="55" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="16"/>
@@ -2848,10 +2888,10 @@
       <c r="O9" s="16"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="16"/>
@@ -2866,40 +2906,40 @@
       <c r="O10" s="16"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="55" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="10"/>
+      <c r="B14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="57"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -2945,18 +2985,18 @@
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="55" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="16"/>
@@ -2987,10 +3027,10 @@
       <c r="O26" s="16"/>
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="10" t="s">
+      <c r="B27" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F27" s="16"/>
@@ -3005,40 +3045,40 @@
       <c r="O27" s="16"/>
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="22" t="s">
+      <c r="B28" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="55" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="B29" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="10" t="s">
+      <c r="B30" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="10"/>
+      <c r="B31" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="54"/>
+      <c r="C32" s="57"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
@@ -3084,18 +3124,18 @@
       </c>
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="10" t="s">
+      <c r="B40" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="22" t="s">
+      <c r="B41" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="55" t="s">
         <v>54</v>
       </c>
       <c r="F41" s="16"/>
@@ -3126,10 +3166,10 @@
       <c r="O42" s="16"/>
     </row>
     <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F43" s="16"/>
@@ -3144,40 +3184,40 @@
       <c r="O43" s="16"/>
     </row>
     <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="22" t="s">
+      <c r="B44" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="55" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="10" t="s">
+      <c r="B46" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="10"/>
+      <c r="B47" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="57"/>
     </row>
     <row r="50" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="21" t="s">
@@ -3220,18 +3260,18 @@
       </c>
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" s="10" t="s">
+      <c r="B56" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="22" t="s">
+      <c r="B57" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="55" t="s">
         <v>54</v>
       </c>
       <c r="F57" s="16"/>
@@ -3262,10 +3302,10 @@
       <c r="O58" s="16"/>
     </row>
     <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="10" t="s">
+      <c r="B59" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="25" t="s">
         <v>44</v>
       </c>
       <c r="F59" s="16"/>
@@ -3280,43 +3320,48 @@
       <c r="O59" s="16"/>
     </row>
     <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" s="22" t="s">
+      <c r="B60" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="55" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" s="10" t="s">
+      <c r="B61" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="10" t="s">
+      <c r="B62" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="10"/>
+      <c r="B63" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="53" t="s">
+      <c r="B64" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C64" s="54"/>
+      <c r="C64" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3324,11 +3369,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
color example 4 packets
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="color code" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="87">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>topicName</t>
   </si>
   <si>
     <t>payload</t>
@@ -239,12 +236,6 @@
     <t>properties</t>
   </si>
   <si>
-    <t xml:space="preserve">  payloadFormat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  contentType</t>
-  </si>
-  <si>
     <t>"application/openc2"</t>
   </si>
   <si>
@@ -257,13 +248,7 @@
     <t>"encoding:json"</t>
   </si>
   <si>
-    <t xml:space="preserve">  userProperty</t>
-  </si>
-  <si>
     <t xml:space="preserve">  maxQoS=2, NL=1, RAP=1, RH=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  flags</t>
   </si>
   <si>
     <t>qos=1, dup=0, retain=0</t>
@@ -1047,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1194,23 +1179,20 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2015,17 +1997,17 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="45" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" s="46" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" s="47" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2075,14 +2057,14 @@
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="34"/>
       <c r="B3" s="39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
@@ -2105,14 +2087,14 @@
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -2121,12 +2103,12 @@
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -2135,14 +2117,14 @@
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="32">
         <v>1</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="43" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -2151,7 +2133,7 @@
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="32">
         <v>1</v>
@@ -2165,7 +2147,7 @@
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
@@ -2179,7 +2161,7 @@
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="25">
         <v>0</v>
@@ -2193,7 +2175,7 @@
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
@@ -2207,7 +2189,7 @@
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C12" s="25">
         <v>0</v>
@@ -2221,7 +2203,7 @@
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
       <c r="B13" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="32">
         <v>0</v>
@@ -2235,10 +2217,10 @@
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -2249,10 +2231,10 @@
     <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
@@ -2263,7 +2245,7 @@
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="49" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C16" s="50">
         <v>300</v>
@@ -2292,10 +2274,10 @@
     </row>
     <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B19" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2308,21 +2290,21 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="10">
         <v>1</v>
@@ -2330,7 +2312,7 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="10">
         <v>1</v>
@@ -2338,7 +2320,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C25" s="25">
         <v>0</v>
@@ -2346,15 +2328,15 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C27" s="25">
         <v>0</v>
@@ -2362,7 +2344,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C28" s="25">
         <v>0</v>
@@ -2370,7 +2352,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
@@ -2378,23 +2360,23 @@
     </row>
     <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="49" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C32" s="50">
         <v>300</v>
@@ -2437,10 +2419,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -2453,7 +2435,7 @@
     </row>
     <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C5" s="10">
         <v>4314</v>
@@ -2461,18 +2443,18 @@
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
@@ -2487,26 +2469,26 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
       <c r="K8" s="17"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
       <c r="N8" s="17"/>
       <c r="O8" s="16"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -2521,37 +2503,37 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="51" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C14" s="24"/>
     </row>
@@ -2566,10 +2548,10 @@
     </row>
     <row r="17" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B17" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -2582,7 +2564,7 @@
     </row>
     <row r="19" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="13">
         <v>4314</v>
@@ -2623,13 +2605,13 @@
     </row>
     <row r="3" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -2642,7 +2624,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="10">
         <v>47826</v>
@@ -2650,66 +2632,66 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="49" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -2726,13 +2708,13 @@
     </row>
     <row r="17" spans="2:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -2745,7 +2727,7 @@
     </row>
     <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="10">
         <v>47826</v>
@@ -2753,7 +2735,7 @@
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="10">
         <v>2</v>
@@ -2761,7 +2743,7 @@
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="10">
         <v>2</v>
@@ -2769,7 +2751,7 @@
     </row>
     <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="10">
         <v>2</v>
@@ -2777,7 +2759,7 @@
     </row>
     <row r="23" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="13">
         <v>2</v>
@@ -2794,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,7 +2790,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2823,10 +2805,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -2839,7 +2821,7 @@
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="22">
         <v>2468</v>
@@ -2847,18 +2829,18 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="55" t="s">
-        <v>18</v>
+        <v>77</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="18"/>
@@ -2873,26 +2855,26 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="10"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
       <c r="K9" s="18"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
       <c r="N9" s="18"/>
       <c r="O9" s="16"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -2907,46 +2889,46 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>45</v>
+        <v>79</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="57"/>
+      <c r="B15" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="55"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
     <row r="18" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C18" s="20"/>
     </row>
@@ -2962,10 +2944,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -2978,7 +2960,7 @@
     </row>
     <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="22">
         <v>3571</v>
@@ -2986,18 +2968,18 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="55" t="s">
-        <v>54</v>
+        <v>77</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="18"/>
@@ -3012,26 +2994,26 @@
     </row>
     <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="10"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
       <c r="N26" s="18"/>
       <c r="O26" s="16"/>
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -3046,46 +3028,46 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>55</v>
+        <v>79</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="57"/>
+      <c r="B32" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="55"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
     </row>
     <row r="34" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C34" s="20"/>
     </row>
@@ -3101,10 +3083,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
@@ -3117,7 +3099,7 @@
     </row>
     <row r="39" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C39" s="22">
         <v>9876</v>
@@ -3125,18 +3107,18 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="55" t="s">
-        <v>54</v>
+        <v>77</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="F41" s="16"/>
       <c r="G41" s="18"/>
@@ -3151,26 +3133,26 @@
     </row>
     <row r="42" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" s="10"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
       <c r="K42" s="18"/>
-      <c r="L42" s="52"/>
-      <c r="M42" s="52"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
       <c r="N42" s="18"/>
       <c r="O42" s="16"/>
     </row>
     <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
@@ -3185,43 +3167,43 @@
     </row>
     <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="55" t="s">
-        <v>55</v>
+        <v>79</v>
+      </c>
+      <c r="C44" s="52" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="57"/>
+      <c r="B48" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="55"/>
     </row>
     <row r="50" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C50" s="20"/>
     </row>
@@ -3237,10 +3219,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
@@ -3253,7 +3235,7 @@
     </row>
     <row r="55" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="22">
         <v>6294</v>
@@ -3261,18 +3243,18 @@
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C57" s="55" t="s">
-        <v>54</v>
+        <v>77</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="18"/>
@@ -3287,26 +3269,26 @@
     </row>
     <row r="58" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C58" s="10"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="52"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="53"/>
       <c r="K58" s="18"/>
-      <c r="L58" s="52"/>
-      <c r="M58" s="52"/>
+      <c r="L58" s="53"/>
+      <c r="M58" s="53"/>
       <c r="N58" s="18"/>
       <c r="O58" s="16"/>
     </row>
     <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
@@ -3321,47 +3303,42 @@
     </row>
     <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="55" t="s">
-        <v>55</v>
+        <v>79</v>
+      </c>
+      <c r="C60" s="52" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="57"/>
+      <c r="B64" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3369,6 +3346,11 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3380,8 +3362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3394,7 +3376,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3409,10 +3391,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -3425,26 +3407,26 @@
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="30">
         <v>62874</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>50</v>
+      <c r="B7" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>65</v>
+      <c r="B8" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>60</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="23"/>
@@ -3459,26 +3441,26 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="30"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
       <c r="N9" s="23"/>
       <c r="O9" s="16"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="56" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>44</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -3492,47 +3474,47 @@
       <c r="O10" s="16"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>45</v>
+      <c r="B11" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>46</v>
+      <c r="B12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>43</v>
+      <c r="B13" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="10"/>
+      <c r="B14" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="54"/>
+      <c r="B15" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="55"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
     <row r="18" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C18" s="20"/>
     </row>
@@ -3548,10 +3530,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -3564,26 +3546,26 @@
     </row>
     <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="30">
         <v>87356</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="56" t="s">
         <v>49</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>54</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="23"/>
@@ -3598,26 +3580,26 @@
     </row>
     <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="30"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
       <c r="K26" s="23"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
       <c r="N26" s="23"/>
       <c r="O26" s="16"/>
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="56" t="s">
         <v>41</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>44</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -3631,40 +3613,40 @@
       <c r="O27" s="16"/>
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>55</v>
+      <c r="B28" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>46</v>
+      <c r="B29" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>43</v>
+      <c r="B30" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="10"/>
+      <c r="B31" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="54"/>
+      <c r="B32" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="55"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>

</xml_diff>

<commit_message>
fix example 3 format glitch
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="color code" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="86">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -758,9 +758,6 @@
       </rPr>
       <t xml:space="preserve"> (r)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  userProperty (r)</t>
   </si>
   <si>
     <r>
@@ -1182,6 +1179,9 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1190,9 +1190,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2473,13 +2470,13 @@
       </c>
       <c r="C8" s="10"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="17"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
       <c r="N8" s="17"/>
       <c r="O8" s="16"/>
     </row>
@@ -2776,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,13 +2856,13 @@
       </c>
       <c r="C9" s="10"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="18"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
       <c r="N9" s="18"/>
       <c r="O9" s="16"/>
     </row>
@@ -2913,15 +2910,15 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="55"/>
+      <c r="C15" s="56"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -2998,13 +2995,13 @@
       </c>
       <c r="C26" s="10"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
       <c r="N26" s="18"/>
       <c r="O26" s="16"/>
     </row>
@@ -3036,7 +3033,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>43</v>
@@ -3052,15 +3049,15 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="55"/>
+      <c r="C32" s="56"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
@@ -3137,13 +3134,13 @@
       </c>
       <c r="C42" s="10"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54"/>
       <c r="K42" s="18"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
       <c r="N42" s="18"/>
       <c r="O42" s="16"/>
     </row>
@@ -3175,7 +3172,7 @@
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>43</v>
@@ -3191,15 +3188,15 @@
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="55"/>
+      <c r="C48" s="56"/>
     </row>
     <row r="50" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="21" t="s">
@@ -3273,13 +3270,13 @@
       </c>
       <c r="C58" s="10"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
+      <c r="I58" s="54"/>
+      <c r="J58" s="54"/>
       <c r="K58" s="18"/>
-      <c r="L58" s="53"/>
-      <c r="M58" s="53"/>
+      <c r="L58" s="54"/>
+      <c r="M58" s="54"/>
       <c r="N58" s="18"/>
       <c r="O58" s="16"/>
     </row>
@@ -3311,7 +3308,7 @@
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>43</v>
@@ -3327,18 +3324,23 @@
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C64" s="55"/>
+      <c r="C64" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3346,11 +3348,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3362,7 +3359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -3417,7 +3414,7 @@
       <c r="B7" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="53" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3425,7 +3422,7 @@
       <c r="B8" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="53" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="16"/>
@@ -3445,13 +3442,13 @@
       </c>
       <c r="C9" s="30"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
       <c r="N9" s="23"/>
       <c r="O9" s="16"/>
     </row>
@@ -3459,7 +3456,7 @@
       <c r="B10" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="53" t="s">
         <v>41</v>
       </c>
       <c r="F10" s="16"/>
@@ -3477,7 +3474,7 @@
       <c r="B11" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3485,7 +3482,7 @@
       <c r="B12" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="53" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3493,21 +3490,21 @@
       <c r="B13" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="53" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="55"/>
+      <c r="C15" s="56"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -3556,7 +3553,7 @@
       <c r="B24" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="53" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3564,7 +3561,7 @@
       <c r="B25" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="C25" s="53" t="s">
         <v>49</v>
       </c>
       <c r="F25" s="16"/>
@@ -3584,13 +3581,13 @@
       </c>
       <c r="C26" s="30"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="23"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
       <c r="N26" s="23"/>
       <c r="O26" s="16"/>
     </row>
@@ -3598,7 +3595,7 @@
       <c r="B27" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="53" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="16"/>
@@ -3616,7 +3613,7 @@
       <c r="B28" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="53" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3624,7 +3621,7 @@
       <c r="B29" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="53" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3632,21 +3629,21 @@
       <c r="B30" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="53" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="55"/>
+      <c r="C32" s="56"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>

</xml_diff>

<commit_message>
use "uuid_1" in example 3
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -275,145 +275,6 @@
     <t>Consumer 3 Response</t>
   </si>
   <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483630,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Producer1@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Consumer3@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"edr","sbom"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483632,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Consumer2@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"slpf","ids"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>]}}}}}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>{"headers":{"request_id":"abc123","created":1610483633,"from":"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>Consumer1@example.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>"slpf"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t>]}}}}}</t>
-    </r>
-  </si>
-  <si>
     <t>Producer request for Consumer APs</t>
   </si>
   <si>
@@ -771,6 +632,145 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> (r)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"uuid_1","created":1610483630,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Producer1@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"request":{"action":"query","target":{"features":["profiles"]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"uuid_1","created":1610483633,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer1@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"slpf"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"uuid_1","created":1610483632,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer2@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"slpf","ids"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{"headers":{"request_id":"uuid_1","created":1610483632,"from":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>Consumer3@example.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"},"body":{"openc2":{"response":{"status":200,"results":{"profiles":[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>"edr","sbom"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>]}}}}}</t>
     </r>
   </si>
 </sst>
@@ -1994,17 +1994,17 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="45" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" s="46" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" s="47" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2084,14 +2084,14 @@
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -2105,7 +2105,7 @@
       <c r="C6" s="32"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="43" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -2144,7 +2144,7 @@
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
@@ -2158,7 +2158,7 @@
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C10" s="25">
         <v>0</v>
@@ -2172,7 +2172,7 @@
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
@@ -2186,7 +2186,7 @@
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12" s="25">
         <v>0</v>
@@ -2214,7 +2214,7 @@
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>46</v>
@@ -2228,7 +2228,7 @@
     <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>9</v>
@@ -2242,7 +2242,7 @@
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C16" s="50">
         <v>300</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>28</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C25" s="25">
         <v>0</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C26" s="48" t="s">
         <v>32</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C27" s="25">
         <v>0</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C28" s="25">
         <v>0</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C32" s="50">
         <v>300</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" s="10">
         <v>4314</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>45</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>12</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>41</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>42</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>43</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>40</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="51" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C14" s="24"/>
     </row>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>17</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>44</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>18</v>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>44</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>12</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>44</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>19</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="49" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>44</v>
@@ -2773,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,7 +2787,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>45</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>17</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>41</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>42</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>43</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>40</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>45</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" s="52" t="s">
         <v>49</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>41</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>50</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>43</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>40</v>
@@ -3049,13 +3049,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C32" s="56"/>
     </row>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C40" s="25" t="s">
         <v>45</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C41" s="52" t="s">
         <v>49</v>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>41</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C44" s="52" t="s">
         <v>50</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>43</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>40</v>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="55" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C48" s="56"/>
     </row>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>45</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>49</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>41</v>
@@ -3300,7 +3300,7 @@
     </row>
     <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C60" s="52" t="s">
         <v>50</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>43</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>40</v>
@@ -3324,23 +3324,18 @@
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="55" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C64" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3348,6 +3343,11 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3373,7 +3373,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C7" s="53" t="s">
         <v>45</v>
@@ -3420,10 +3420,10 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="23"/>
@@ -3454,7 +3454,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>41</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C11" s="53" t="s">
         <v>42</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C12" s="53" t="s">
         <v>43</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>40</v>
@@ -3496,13 +3496,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="18" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="20"/>
     </row>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C24" s="53" t="s">
         <v>45</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" s="53" t="s">
         <v>49</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C27" s="53" t="s">
         <v>41</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C28" s="53" t="s">
         <v>50</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C29" s="53" t="s">
         <v>43</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C30" s="53" t="s">
         <v>40</v>
@@ -3635,13 +3635,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C32" s="56"/>
     </row>

</xml_diff>

<commit_message>
use "uuid_2" in example 4
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="color code" sheetId="7" r:id="rId1"/>
@@ -299,12 +299,6 @@
     <t>"oc2/cmd/splf"</t>
   </si>
   <si>
-    <t>{"headers":{"request_id":"ghk479","created":1610483630,"from":"Producer1@example.com"},"body":{"openc2":{"request":{"action":"deny","target":{"ipv4_connection":{"protocol":"tcp","src_addr":"1.2.3.4","src_port":10996,"dst_addr":"198.2.3.4","dst_port":80}},"args":{"start_time":1534775460000,"duration":500,"response_requested":"ack","slpf":{"drop_process":"none"}},"actuator":{"slpf":{"asset_id":"30"}}}}}}</t>
-  </si>
-  <si>
-    <t>{"headers":{"request_id":"ghk479","created":1610483633,"from":"Consumer1@example.com"},"body":{"openc2":{"response":{"status":102}}}}</t>
-  </si>
-  <si>
     <t>Consumer 1 Response to `deny` Request</t>
   </si>
   <si>
@@ -772,6 +766,12 @@
       </rPr>
       <t>]}}}}}</t>
     </r>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"uuid_2","created":1610483630,"from":"Producer1@example.com"},"body":{"openc2":{"request":{"action":"deny","target":{"ipv4_connection":{"protocol":"tcp","src_addr":"1.2.3.4","src_port":10996,"dst_addr":"198.2.3.4","dst_port":80}},"args":{"start_time":1534775460000,"duration":500,"response_requested":"ack","slpf":{"drop_process":"none"}},"actuator":{"slpf":{"asset_id":"30"}}}}}}</t>
+  </si>
+  <si>
+    <t>{"headers":{"request_id":"uuid_2","created":1610483633,"from":"Consumer1@example.com"},"body":{"openc2":{"response":{"status":102}}}}</t>
   </si>
 </sst>
 </file>
@@ -1994,17 +1994,17 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" s="46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" s="47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2084,14 +2084,14 @@
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -2105,7 +2105,7 @@
       <c r="C6" s="32"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -2144,7 +2144,7 @@
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
@@ -2158,7 +2158,7 @@
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="25">
         <v>0</v>
@@ -2172,7 +2172,7 @@
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
@@ -2186,7 +2186,7 @@
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="25">
         <v>0</v>
@@ -2214,7 +2214,7 @@
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>46</v>
@@ -2228,7 +2228,7 @@
     <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>9</v>
@@ -2242,7 +2242,7 @@
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="50">
         <v>300</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>28</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="25">
         <v>0</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C26" s="48" t="s">
         <v>32</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="25">
         <v>0</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="25">
         <v>0</v>
@@ -2373,7 +2373,7 @@
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" s="50">
         <v>300</v>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>45</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>12</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>41</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>42</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>43</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>40</v>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="51" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="24"/>
     </row>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>17</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>44</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>18</v>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>44</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>12</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>44</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>19</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="49" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>44</v>
@@ -2773,7 +2773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>45</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>17</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>41</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>42</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>43</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>40</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>45</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="52" t="s">
         <v>49</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>41</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>50</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>43</v>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>40</v>
@@ -3049,13 +3049,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C32" s="56"/>
     </row>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" s="25" t="s">
         <v>45</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C41" s="52" t="s">
         <v>49</v>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>41</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C44" s="52" t="s">
         <v>50</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>43</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>40</v>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="55" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C48" s="56"/>
     </row>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>45</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>49</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>41</v>
@@ -3300,7 +3300,7 @@
     </row>
     <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C60" s="52" t="s">
         <v>50</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>43</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>40</v>
@@ -3324,18 +3324,23 @@
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C64" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3343,11 +3348,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3359,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="53" t="s">
         <v>45</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="53" t="s">
         <v>56</v>
@@ -3454,7 +3454,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>41</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="53" t="s">
         <v>42</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="53" t="s">
         <v>43</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>40</v>
@@ -3496,13 +3496,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="18" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C18" s="20"/>
     </row>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="53" t="s">
         <v>45</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="53" t="s">
         <v>49</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="53" t="s">
         <v>41</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="53" t="s">
         <v>50</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="53" t="s">
         <v>43</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="53" t="s">
         <v>40</v>
@@ -3635,13 +3635,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C32" s="56"/>
     </row>

</xml_diff>

<commit_message>
correct color code error in example 2 packet
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="color code" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="85">
   <si>
     <t>MQTT-Packet</t>
   </si>
@@ -497,20 +497,6 @@
         <family val="3"/>
       </rPr>
       <t xml:space="preserve"> (r)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  flags</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> (s)</t>
     </r>
   </si>
   <si>
@@ -2392,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,16 +2425,16 @@
       </c>
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="28" t="s">
+      <c r="B6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>12</v>
@@ -2482,7 +2468,7 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>41</v>
@@ -2500,7 +2486,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>42</v>
@@ -2508,7 +2494,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>43</v>
@@ -2516,7 +2502,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>40</v>
@@ -2530,7 +2516,7 @@
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="24"/>
     </row>
@@ -2629,7 +2615,7 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>17</v>
@@ -2637,7 +2623,7 @@
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>44</v>
@@ -2645,7 +2631,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>18</v>
@@ -2653,7 +2639,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>44</v>
@@ -2661,7 +2647,7 @@
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>12</v>
@@ -2669,7 +2655,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>44</v>
@@ -2677,7 +2663,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>19</v>
@@ -2685,7 +2671,7 @@
     </row>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>44</v>
@@ -2826,7 +2812,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>45</v>
@@ -2834,7 +2820,7 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>17</v>
@@ -2868,7 +2854,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>41</v>
@@ -2886,7 +2872,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>42</v>
@@ -2894,7 +2880,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>43</v>
@@ -2902,7 +2888,7 @@
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>40</v>
@@ -2910,13 +2896,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -2965,7 +2951,7 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>45</v>
@@ -2973,7 +2959,7 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="52" t="s">
         <v>49</v>
@@ -3007,7 +2993,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>41</v>
@@ -3025,7 +3011,7 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>50</v>
@@ -3033,7 +3019,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>43</v>
@@ -3041,7 +3027,7 @@
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>40</v>
@@ -3049,13 +3035,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="56"/>
     </row>
@@ -3104,7 +3090,7 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="25" t="s">
         <v>45</v>
@@ -3112,7 +3098,7 @@
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C41" s="52" t="s">
         <v>49</v>
@@ -3146,7 +3132,7 @@
     </row>
     <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>41</v>
@@ -3164,7 +3150,7 @@
     </row>
     <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="52" t="s">
         <v>50</v>
@@ -3172,7 +3158,7 @@
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>43</v>
@@ -3180,7 +3166,7 @@
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>40</v>
@@ -3188,13 +3174,13 @@
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" s="56"/>
     </row>
@@ -3240,7 +3226,7 @@
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>45</v>
@@ -3248,7 +3234,7 @@
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="52" t="s">
         <v>49</v>
@@ -3282,7 +3268,7 @@
     </row>
     <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>41</v>
@@ -3300,7 +3286,7 @@
     </row>
     <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C60" s="52" t="s">
         <v>50</v>
@@ -3308,7 +3294,7 @@
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>43</v>
@@ -3316,7 +3302,7 @@
     </row>
     <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>40</v>
@@ -3324,23 +3310,18 @@
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3348,6 +3329,11 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3359,7 +3345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
@@ -3412,7 +3398,7 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="53" t="s">
         <v>45</v>
@@ -3420,7 +3406,7 @@
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="53" t="s">
         <v>56</v>
@@ -3454,7 +3440,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>41</v>
@@ -3472,7 +3458,7 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="53" t="s">
         <v>42</v>
@@ -3480,7 +3466,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="53" t="s">
         <v>43</v>
@@ -3488,7 +3474,7 @@
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>40</v>
@@ -3496,13 +3482,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -3551,7 +3537,7 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="53" t="s">
         <v>45</v>
@@ -3559,7 +3545,7 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="53" t="s">
         <v>49</v>
@@ -3593,7 +3579,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="53" t="s">
         <v>41</v>
@@ -3611,7 +3597,7 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="53" t="s">
         <v>50</v>
@@ -3619,7 +3605,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="53" t="s">
         <v>43</v>
@@ -3627,7 +3613,7 @@
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="53" t="s">
         <v>40</v>
@@ -3635,13 +3621,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="56"/>
     </row>

</xml_diff>

<commit_message>
Update example graphics, source
</commit_message>
<xml_diff>
--- a/sources/SampleMessages.xlsx
+++ b/sources/SampleMessages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="683"/>
   </bookViews>
   <sheets>
     <sheet name="color code" sheetId="7" r:id="rId1"/>
@@ -242,12 +242,6 @@
     <t>1 (UTF-8 string)</t>
   </si>
   <si>
-    <t>"msgType:req"</t>
-  </si>
-  <si>
-    <t>"encoding:json"</t>
-  </si>
-  <si>
     <t xml:space="preserve">  maxQoS=2, NL=1, RAP=1, RH=0</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
   </si>
   <si>
     <t>"oc2/rsp"</t>
-  </si>
-  <si>
-    <t>"msgType:rsp"</t>
   </si>
   <si>
     <t>Consumer 2 Response</t>
@@ -758,6 +749,15 @@
   </si>
   <si>
     <t>{"headers":{"request_id":"uuid_2","created":1610483633,"from":"Consumer1@example.com"},"body":{"openc2":{"response":{"status":102}}}}</t>
+  </si>
+  <si>
+    <t>"msgType":"req"</t>
+  </si>
+  <si>
+    <t>"encoding":"json"</t>
+  </si>
+  <si>
+    <t>"msgType":"rsp"</t>
   </si>
 </sst>
 </file>
@@ -1969,7 +1969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -1980,17 +1980,17 @@
   <sheetData>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" s="45" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" s="46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" s="47" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2070,14 +2070,14 @@
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
@@ -2091,7 +2091,7 @@
       <c r="C6" s="32"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="43" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -2130,7 +2130,7 @@
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="25">
         <v>0</v>
@@ -2144,7 +2144,7 @@
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="25">
         <v>0</v>
@@ -2158,7 +2158,7 @@
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
@@ -2172,7 +2172,7 @@
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="25">
         <v>0</v>
@@ -2200,10 +2200,10 @@
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -2214,7 +2214,7 @@
     <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="34"/>
       <c r="B15" s="31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>9</v>
@@ -2228,7 +2228,7 @@
     <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34"/>
       <c r="B16" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" s="50">
         <v>300</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>28</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="25">
         <v>0</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" s="48" t="s">
         <v>32</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="25">
         <v>0</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="25">
         <v>0</v>
@@ -2346,7 +2346,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
@@ -2359,7 +2359,7 @@
     </row>
     <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C32" s="50">
         <v>300</v>
@@ -2378,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,7 +2418,7 @@
     </row>
     <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="10">
         <v>4314</v>
@@ -2426,15 +2426,15 @@
     </row>
     <row r="6" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>12</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>41</v>
@@ -2486,23 +2486,23 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>40</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="51" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C14" s="24"/>
     </row>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>17</v>
@@ -2623,15 +2623,15 @@
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>18</v>
@@ -2639,15 +2639,15 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>12</v>
@@ -2655,15 +2655,15 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>19</v>
@@ -2671,10 +2671,10 @@
     </row>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -2759,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="U61" sqref="U61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,7 +2773,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2812,15 +2812,15 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>17</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>41</v>
@@ -2872,23 +2872,23 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>40</v>
@@ -2896,13 +2896,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="18" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="20"/>
     </row>
@@ -2951,18 +2951,18 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="18"/>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>41</v>
@@ -3011,23 +3011,23 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>40</v>
@@ -3035,13 +3035,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C32" s="56"/>
     </row>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="34" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" s="20"/>
     </row>
@@ -3090,18 +3090,18 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F41" s="16"/>
       <c r="G41" s="18"/>
@@ -3132,7 +3132,7 @@
     </row>
     <row r="43" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>41</v>
@@ -3150,23 +3150,23 @@
     </row>
     <row r="44" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>40</v>
@@ -3174,19 +3174,19 @@
     </row>
     <row r="47" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C48" s="56"/>
     </row>
     <row r="50" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C50" s="20"/>
     </row>
@@ -3226,18 +3226,18 @@
     </row>
     <row r="56" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C57" s="52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="18"/>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="59" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>41</v>
@@ -3286,23 +3286,23 @@
     </row>
     <row r="60" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C60" s="52" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>40</v>
@@ -3310,18 +3310,23 @@
     </row>
     <row r="63" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C64" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="G42:J42"/>
@@ -3329,11 +3334,6 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="G58:J58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="L26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3346,7 +3346,7 @@
   <dimension ref="B1:O33"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,7 +3359,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3398,18 +3398,18 @@
     </row>
     <row r="7" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="23"/>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>41</v>
@@ -3458,23 +3458,23 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>40</v>
@@ -3482,13 +3482,13 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="25"/>
     </row>
     <row r="15" spans="2:15" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C15" s="56"/>
     </row>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="18" spans="2:15" s="19" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C18" s="20"/>
     </row>
@@ -3537,18 +3537,18 @@
     </row>
     <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="23"/>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="27" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C27" s="53" t="s">
         <v>41</v>
@@ -3597,23 +3597,23 @@
     </row>
     <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C28" s="53" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C29" s="53" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C30" s="53" t="s">
         <v>40</v>
@@ -3621,13 +3621,13 @@
     </row>
     <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" s="25"/>
     </row>
     <row r="32" spans="2:15" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" s="56"/>
     </row>

</xml_diff>